<commit_message>
analytical model scritpts and optimize split
</commit_message>
<xml_diff>
--- a/optimize_split/real_data/resnet101_CIFAR.xlsx
+++ b/optimize_split/real_data/resnet101_CIFAR.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Documents/git_repos/Pipelined-Federeated-Split-Learning/optimize_split/real_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E93A48-9F8E-C24D-932B-DCCD69074F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FCFC1D-EB21-F54E-BF39-67764E48C395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="500" windowWidth="14880" windowHeight="17500" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="10000" windowHeight="17500" activeTab="7" xr2:uid="{7935258D-7BA1-BE4D-B533-9C0418764F7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="VM" sheetId="1" r:id="rId1"/>
-    <sheet name="laptop" sheetId="5" r:id="rId2"/>
-    <sheet name="d1" sheetId="2" r:id="rId3"/>
-    <sheet name="d2" sheetId="3" r:id="rId4"/>
-    <sheet name="jetson-cpu" sheetId="7" r:id="rId5"/>
-    <sheet name="jetson-gpu" sheetId="8" r:id="rId6"/>
-    <sheet name="memory" sheetId="6" r:id="rId7"/>
+    <sheet name="VM" sheetId="9" r:id="rId1"/>
+    <sheet name="VM__" sheetId="1" r:id="rId2"/>
+    <sheet name="laptop" sheetId="5" r:id="rId3"/>
+    <sheet name="d1" sheetId="2" r:id="rId4"/>
+    <sheet name="d2" sheetId="3" r:id="rId5"/>
+    <sheet name="jetson-cpu" sheetId="7" r:id="rId6"/>
+    <sheet name="jetson-gpu" sheetId="8" r:id="rId7"/>
+    <sheet name="memory" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,12 +66,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF833C0C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,10 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,11 +417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3907375A-5822-0A45-92DF-EC04FBC81381}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AB92C7-4D4A-ED41-BA3A-EEA39EE3C10A}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A4" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,6 +436,10 @@
       <c r="C1" s="1">
         <v>0</v>
       </c>
+      <c r="E1">
+        <f>A1+B1+C1</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -432,6 +451,10 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E37" si="0">A2+B2+C2</f>
+        <v>4.4615400000000003</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -443,6 +466,10 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>28.692279999999997</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -454,6 +481,10 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>27.923079999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -465,6 +496,10 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>28.23076</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -476,6 +511,10 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>29.999980000000001</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
@@ -489,6 +528,10 @@
       <c r="C7" s="1">
         <v>0</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>27.53848</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
@@ -502,6 +545,10 @@
       <c r="C8" s="1">
         <v>0</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>27.53848</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -513,6 +560,10 @@
       <c r="C9" s="1">
         <v>0</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>27.692279999999997</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -524,6 +575,10 @@
       <c r="C10" s="1">
         <v>1.0769200000000001</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>53.769220000000004</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -535,6 +590,10 @@
       <c r="C11" s="1">
         <v>1.0769200000000001</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>51.846150000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -546,6 +605,10 @@
       <c r="C12" s="1">
         <v>1.0769200000000001</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>51.076950000000004</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -557,6 +620,10 @@
       <c r="C13" s="1">
         <v>1.0769200000000001</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>51.76925</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -568,6 +635,10 @@
       <c r="C14" s="1">
         <v>1.0769200000000001</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>51.692350000000005</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -579,6 +650,10 @@
       <c r="C15" s="1">
         <v>1.0769200000000001</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>51.230730000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -590,8 +665,12 @@
       <c r="C16" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>51.846200000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8.7692300000000003</v>
       </c>
@@ -601,8 +680,12 @@
       <c r="C17" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>51.538450000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>8.6923100000000009</v>
       </c>
@@ -612,8 +695,12 @@
       <c r="C18" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>51.615430000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>8.6923100000000009</v>
       </c>
@@ -623,8 +710,12 @@
       <c r="C19" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>52.230730000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>8.8461499999999997</v>
       </c>
@@ -634,8 +725,12 @@
       <c r="C20" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>53.07687</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -645,8 +740,12 @@
       <c r="C21" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>52.538420000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>8.9230800000000006</v>
       </c>
@@ -656,8 +755,12 @@
       <c r="C22" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>54.076900000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>8.8461499999999997</v>
       </c>
@@ -667,8 +770,12 @@
       <c r="C23" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>53.23077</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>8.7692300000000003</v>
       </c>
@@ -678,8 +785,12 @@
       <c r="C24" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>53.999949999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>8.8461499999999997</v>
       </c>
@@ -689,8 +800,12 @@
       <c r="C25" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>53.769270000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>8.8461499999999997</v>
       </c>
@@ -700,8 +815,12 @@
       <c r="C26" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>54.384570000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>9.4615399999999994</v>
       </c>
@@ -711,8 +830,12 @@
       <c r="C27" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>54.92306</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>9.4615399999999994</v>
       </c>
@@ -722,8 +845,12 @@
       <c r="C28" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>55.538460000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>9.5384600000000006</v>
       </c>
@@ -733,8 +860,12 @@
       <c r="C29" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>55.076880000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>9.4615399999999994</v>
       </c>
@@ -744,8 +875,12 @@
       <c r="C30" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>54.769260000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>9.4615399999999994</v>
       </c>
@@ -755,8 +890,12 @@
       <c r="C31" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>54.538460000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>9.7692300000000003</v>
       </c>
@@ -766,8 +905,12 @@
       <c r="C32" s="1">
         <v>1.0769200000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>55.307650000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>16.923100000000002</v>
       </c>
@@ -777,8 +920,12 @@
       <c r="C33" s="1">
         <v>3.4615399999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>175.46164000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>12</v>
       </c>
@@ -788,8 +935,12 @@
       <c r="C34" s="1">
         <v>3.8461500000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>194.76915</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>12</v>
       </c>
@@ -799,8 +950,12 @@
       <c r="C35" s="1">
         <v>3.7692299999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>192.84622999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -810,8 +965,12 @@
       <c r="C36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -819,6 +978,10 @@
         <v>0</v>
       </c>
       <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -828,6 +991,1036 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3907375A-5822-0A45-92DF-EC04FBC81381}">
+  <dimension ref="A1:Q40"/>
+  <sheetViews>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="E35" sqref="C32:E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>3.2307700000000001</v>
+      </c>
+      <c r="B1" s="1">
+        <v>5.7692300000000003</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <f>SUM(A1:C1)</f>
+        <v>9</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>3.30769</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.15385</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E37" si="0">SUM(A2:C2)</f>
+        <v>4.4615400000000003</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>6.61538</v>
+      </c>
+      <c r="B3" s="1">
+        <v>22.076899999999998</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>28.692279999999997</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>6.61538</v>
+      </c>
+      <c r="B4" s="1">
+        <v>21.307700000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>27.923079999999999</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>6.5384599999999997</v>
+      </c>
+      <c r="B5" s="1">
+        <v>21.692299999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>28.23076</v>
+      </c>
+      <c r="G5">
+        <f>SUM(E2:E18)</f>
+        <v>668.46161000000006</v>
+      </c>
+      <c r="H5">
+        <f>SUM(A2:A18)</f>
+        <v>130.76918000000001</v>
+      </c>
+      <c r="I5">
+        <f>SUM(B2:C18)</f>
+        <v>537.69242999999983</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5">
+        <f>SUM(E2:E14)</f>
+        <v>462.23080000000004</v>
+      </c>
+      <c r="L5">
+        <f>SUM(A2:A14)</f>
+        <v>95.692250000000001</v>
+      </c>
+      <c r="M5">
+        <f>SUM(B2:C14)</f>
+        <v>366.53854999999993</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5">
+        <f>SUM(E2:E13)</f>
+        <v>410.53845000000001</v>
+      </c>
+      <c r="P5">
+        <f>SUM(A2:A13)</f>
+        <v>86.923020000000008</v>
+      </c>
+      <c r="Q5">
+        <f>SUM(B2:C13)</f>
+        <v>323.61542999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>7.61538</v>
+      </c>
+      <c r="B6" s="1">
+        <v>22.384599999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>29.999980000000001</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <f>SUM(E19:E30)</f>
+        <v>647.61514</v>
+      </c>
+      <c r="H6">
+        <f>SUM(A19:A30)</f>
+        <v>108.6923</v>
+      </c>
+      <c r="I6">
+        <f>SUM(B19:C30)</f>
+        <v>538.92283999999984</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6">
+        <f>SUM(E15:E23)</f>
+        <v>471.3845</v>
+      </c>
+      <c r="L6">
+        <f>SUM(A15:A23)</f>
+        <v>79.384619999999998</v>
+      </c>
+      <c r="M6">
+        <f>SUM(B15:C23)</f>
+        <v>391.99987999999996</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6">
+        <f>SUM(E14:E21)</f>
+        <v>415.76918000000001</v>
+      </c>
+      <c r="P6">
+        <f>SUM(A14:A21)</f>
+        <v>70.384619999999998</v>
+      </c>
+      <c r="Q6">
+        <f>SUM(B14:C21)</f>
+        <v>345.38455999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6.61538</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20.923100000000002</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>27.53848</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <f>SUM(E31:E36)</f>
+        <v>672.92313000000001</v>
+      </c>
+      <c r="H7">
+        <f>SUM(A31:A36)</f>
+        <v>60.153869999999998</v>
+      </c>
+      <c r="I7">
+        <f>SUM(B31:C36)</f>
+        <v>612.76926000000003</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7">
+        <f>SUM(E24:E32)</f>
+        <v>492.30756000000002</v>
+      </c>
+      <c r="L7">
+        <f>SUM(A24:A32)</f>
+        <v>83.615380000000016</v>
+      </c>
+      <c r="M7">
+        <f>SUM(B24:C32)</f>
+        <v>408.69217999999989</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7">
+        <f>SUM(E22:E27)</f>
+        <v>324.38452000000001</v>
+      </c>
+      <c r="P7">
+        <f>SUM(A22:A27)</f>
+        <v>53.692300000000003</v>
+      </c>
+      <c r="Q7">
+        <f>SUM(B22:C27)</f>
+        <v>270.69221999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6.61538</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20.923100000000002</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>27.53848</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8">
+        <f>SUM(E33:E36)</f>
+        <v>563.07701999999995</v>
+      </c>
+      <c r="L8">
+        <f>SUM(A33:A36)</f>
+        <v>40.923100000000005</v>
+      </c>
+      <c r="M8">
+        <f>SUM(B33:C36)</f>
+        <v>522.15392000000008</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8">
+        <f>SUM(E28:E33)</f>
+        <v>450.69235000000003</v>
+      </c>
+      <c r="P8">
+        <f>SUM(A28:A33)</f>
+        <v>64.615409999999997</v>
+      </c>
+      <c r="Q8">
+        <f>SUM(B28:C33)</f>
+        <v>386.07694000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6.61538</v>
+      </c>
+      <c r="B9" s="1">
+        <v>21.076899999999998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>27.692279999999997</v>
+      </c>
+      <c r="H9">
+        <f>MAX(H6:H7)</f>
+        <v>108.6923</v>
+      </c>
+      <c r="I9">
+        <f>MAX(I6:I7)</f>
+        <v>612.76926000000003</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="N9" s="4"/>
+      <c r="O9">
+        <f>SUM(E34:E36)</f>
+        <v>387.61537999999996</v>
+      </c>
+      <c r="P9">
+        <f>SUM(A34:A36)</f>
+        <v>24</v>
+      </c>
+      <c r="Q9">
+        <f>SUM(B34:C36)</f>
+        <v>363.61537999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>10.0769</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42.615400000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>53.769220000000004</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H9:I9)</f>
+        <v>721.46156000000008</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="L10">
+        <f>MAX(L5:L8)</f>
+        <v>95.692250000000001</v>
+      </c>
+      <c r="M10">
+        <f>MAX(M5:M8)</f>
+        <v>522.15392000000008</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>8.7692300000000003</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>51.846150000000002</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="L11">
+        <f>SUM(L10:M10)</f>
+        <v>617.84617000000003</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="P11">
+        <f>MAX(P5:P9)</f>
+        <v>86.923020000000008</v>
+      </c>
+      <c r="Q11">
+        <f>MAX(Q5:Q9)</f>
+        <v>386.07694000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>8.7692300000000003</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41.230800000000002</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>51.076950000000004</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="N12" s="4"/>
+      <c r="P12">
+        <f>SUM(P11:Q11)</f>
+        <v>472.99996000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>8.7692300000000003</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41.923099999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>51.76925</v>
+      </c>
+      <c r="G13">
+        <f>SUM(E2:E13)</f>
+        <v>410.53845000000001</v>
+      </c>
+      <c r="H13">
+        <f>SUM(A2:A13)</f>
+        <v>86.923020000000008</v>
+      </c>
+      <c r="I13">
+        <f>SUM(B2:C13)</f>
+        <v>323.61542999999995</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13">
+        <f>SUM(E2:E12)</f>
+        <v>358.76920000000001</v>
+      </c>
+      <c r="L13">
+        <f>SUM(A2:A12)</f>
+        <v>78.153790000000015</v>
+      </c>
+      <c r="M13">
+        <f>SUM(B2:C12)</f>
+        <v>280.61541</v>
+      </c>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>8.7692300000000003</v>
+      </c>
+      <c r="B14" s="1">
+        <v>41.846200000000003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E14">
+        <f>SUM(A14:C14)</f>
+        <v>51.692350000000005</v>
+      </c>
+      <c r="G14">
+        <f>SUM(E14:E25)</f>
+        <v>630.84607000000005</v>
+      </c>
+      <c r="H14">
+        <f>SUM(A14:A25)</f>
+        <v>105.76922999999999</v>
+      </c>
+      <c r="I14">
+        <f>SUM(B14:C25)</f>
+        <v>525.07683999999983</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14">
+        <f>SUM(E13:E21)</f>
+        <v>467.53842999999995</v>
+      </c>
+      <c r="L14">
+        <f>SUM(A13:A21)</f>
+        <v>79.153849999999991</v>
+      </c>
+      <c r="M14">
+        <f>SUM(B13:C21)</f>
+        <v>388.38457999999986</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="P14">
+        <f>SUM(A2:A8)</f>
+        <v>43.923050000000003</v>
+      </c>
+      <c r="Q14">
+        <f>SUM(B2:C8)</f>
+        <v>130.46155000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>8.6923100000000009</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41.461500000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>51.230730000000001</v>
+      </c>
+      <c r="G15">
+        <f>SUM(E26:E36)</f>
+        <v>947.61536000000001</v>
+      </c>
+      <c r="H15">
+        <f>SUM(A26:A36)</f>
+        <v>106.92310000000001</v>
+      </c>
+      <c r="I15">
+        <f>SUM(B26:C36)</f>
+        <v>840.69225999999992</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15">
+        <f>SUM(E22:E30)</f>
+        <v>489.76912000000004</v>
+      </c>
+      <c r="L15">
+        <f>SUM(A22:A30)</f>
+        <v>82.153840000000002</v>
+      </c>
+      <c r="M15">
+        <f>SUM(B22:C30)</f>
+        <v>407.61527999999987</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="P15">
+        <f>SUM(A9:A15)</f>
+        <v>60.461509999999997</v>
+      </c>
+      <c r="Q15">
+        <f>SUM(B9:C15)</f>
+        <v>278.61541999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>8.9230800000000006</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41.846200000000003</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>51.846200000000003</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16">
+        <f>SUM(E29:E36)</f>
+        <v>782.76927000000001</v>
+      </c>
+      <c r="L16">
+        <f>SUM(A31:A36)</f>
+        <v>60.153869999999998</v>
+      </c>
+      <c r="M16">
+        <f>SUM(B31:C36)</f>
+        <v>612.76926000000003</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="P16">
+        <f>SUM(A16:A22)</f>
+        <v>61.846159999999998</v>
+      </c>
+      <c r="Q16">
+        <f>SUM(B16:C22)</f>
+        <v>305.07683999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>8.7692300000000003</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41.692300000000003</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>51.538450000000005</v>
+      </c>
+      <c r="H17">
+        <f>MAX(H14:H15)</f>
+        <v>106.92310000000001</v>
+      </c>
+      <c r="I17">
+        <f>MAX(I14:I15)</f>
+        <v>840.69225999999992</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="N17" s="4"/>
+      <c r="P17">
+        <f>SUM(A23:A29)</f>
+        <v>63.769220000000004</v>
+      </c>
+      <c r="Q17">
+        <f>SUM(B23:C29)</f>
+        <v>317.15373999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>8.6923100000000009</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41.846200000000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>51.615430000000003</v>
+      </c>
+      <c r="H18">
+        <f>SUM(H17:I17)</f>
+        <v>947.6153599999999</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="L18">
+        <f>MAX(L13:L16)</f>
+        <v>82.153840000000002</v>
+      </c>
+      <c r="M18">
+        <f>MAX(M13:M16)</f>
+        <v>612.76926000000003</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="P18">
+        <f>SUM(A30:A36)</f>
+        <v>69.615409999999997</v>
+      </c>
+      <c r="Q18">
+        <f>SUM(B30:C36)</f>
+        <v>658.07697999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>8.6923100000000009</v>
+      </c>
+      <c r="B19" s="1">
+        <v>42.461500000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>52.230730000000001</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="L19">
+        <f>SUM(L18:M18)</f>
+        <v>694.92309999999998</v>
+      </c>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>8.8461499999999997</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43.153799999999997</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>53.07687</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="N20" s="4"/>
+      <c r="P20">
+        <f>MAX(P14:P18)</f>
+        <v>69.615409999999997</v>
+      </c>
+      <c r="Q20">
+        <f>MAX(Q14:Q18)</f>
+        <v>658.07697999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>42.461500000000001</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>52.538420000000002</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="N21" s="4"/>
+      <c r="P21">
+        <f>SUM(P20:Q20)</f>
+        <v>727.69238999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>8.9230800000000006</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44.076900000000002</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>54.076900000000002</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>8.8461499999999997</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43.307699999999997</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>53.23077</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>8.7692300000000003</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44.153799999999997</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>53.999949999999998</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>8.8461499999999997</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43.846200000000003</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>53.769270000000006</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>8.8461499999999997</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44.461500000000001</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>54.384570000000004</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>9.4615399999999994</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44.384599999999999</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>54.92306</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>9.4615399999999994</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>55.538460000000001</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>9.5384600000000006</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44.461500000000001</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>55.076880000000003</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>9.4615399999999994</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44.230800000000002</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>54.769260000000003</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>9.4615399999999994</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>54.538460000000001</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>9.7692300000000003</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44.461500000000001</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.0769200000000001</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>55.307650000000002</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>16.923100000000002</v>
+      </c>
+      <c r="B33" s="1">
+        <v>155.077</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3.4615399999999998</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>175.46164000000002</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1">
+        <v>178.923</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3.8461500000000002</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>194.76915</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1">
+        <v>177.077</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3.7692299999999999</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>192.84622999999999</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="N35" s="4"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J38" s="3"/>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <f>SUM(E2:E36)</f>
+        <v>1988.9998800000003</v>
+      </c>
+      <c r="G39">
+        <f>E39/3</f>
+        <v>662.9999600000001</v>
+      </c>
+      <c r="J39" s="3"/>
+      <c r="K39">
+        <f>E39/4</f>
+        <v>497.24997000000008</v>
+      </c>
+      <c r="N39" s="4"/>
+      <c r="O39">
+        <f>E39/5</f>
+        <v>397.79997600000007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <f>COUNT(E2:E36)</f>
+        <v>35</v>
+      </c>
+      <c r="G40">
+        <f>E40/3</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="J40" s="3"/>
+      <c r="K40">
+        <f>E40/4</f>
+        <v>8.75</v>
+      </c>
+      <c r="N40" s="4"/>
+      <c r="O40">
+        <f>E40/5</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF728E79-D3DB-1040-8D51-06514020BC7B}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -1249,7 +2442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3ECEB3-F06F-004D-B5F3-5A36A880D2D3}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -1671,7 +2864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCCCD9C-B55F-B540-99FD-13E476D49529}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -2094,7 +3287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661B018C-5EB8-4041-892E-650D89DBC4B5}">
   <dimension ref="A1:C40"/>
   <sheetViews>
@@ -2519,7 +3712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA781742-6964-264E-BD04-C0478125399C}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -2941,317 +4134,472 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB2EFC7-8096-8542-AF66-11F811B1415F}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>8193.568359375</v>
       </c>
       <c r="B1" s="1">
         <v>39.435546875</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1">
+        <f t="shared" ref="D1:D36" si="0">(A1+B1)/1024</f>
+        <v>8.0400428771972656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2049.568359375</v>
       </c>
       <c r="B2" s="1">
         <v>5.353515625</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>2.0067596435546875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2049.568359375</v>
       </c>
       <c r="B3" s="1">
         <v>298.00390625</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>2.2925510406494141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2049.568359375</v>
       </c>
       <c r="B4" s="1">
         <v>298.00390625</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.2925510406494141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2049.568359375</v>
       </c>
       <c r="B5" s="1">
         <v>298.00390625</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2.2925510406494141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1025.568359375</v>
       </c>
       <c r="B6" s="1">
         <v>1169.599609375</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.1437187194824219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1025.568359375</v>
       </c>
       <c r="B7" s="1">
         <v>1164.00390625</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2.1382541656494141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1025.568359375</v>
       </c>
       <c r="B8" s="1">
         <v>1164.00390625</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.1382541656494141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1025.568359375</v>
       </c>
       <c r="B9" s="1">
         <v>1164.00390625</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.1382541656494141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B10" s="1">
         <v>4631.599609375</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>5.0245780944824219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B11" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B12" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B13" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B14" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B15" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B16" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B17" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B18" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B19" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B20" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B21" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B22" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B23" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B24" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B25" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B26" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B27" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B28" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B29" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B30" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B31" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>513.568359375</v>
       </c>
       <c r="B32" s="1">
         <v>4624.00390625</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>5.0171604156494141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>257.568359375</v>
       </c>
       <c r="B33" s="1">
         <v>18467.599609375</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>18.286296844482422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>257.568359375</v>
       </c>
       <c r="B34" s="1">
         <v>18456.00390625</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>18.274972915649414</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>257.568359375</v>
       </c>
       <c r="B35" s="1">
         <v>18456.00390625</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>18.274972915649414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>257.568359375</v>
       </c>
       <c r="B36" s="1">
         <v>1.880859375</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0.25336837768554688</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>6.505859375</v>
       </c>
       <c r="B37" s="1">
         <v>22.435546875</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <f>(A37+B37)/1024</f>
+        <v>2.8263092041015625E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <f>SUM(D1:D37)</f>
+        <v>196.0029182434082</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>